<commit_message>
Excels arreglados y nuevas inferencias de metastasis, supervivencia y recidivas realizadas
</commit_message>
<xml_diff>
--- a/patient_status/distant_metastasis/inference/data/test_data&models/inference_inibica_metastasis.xlsx
+++ b/patient_status/distant_metastasis/inference/data/test_data&models/inference_inibica_metastasis.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$LG$110</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1662,9 +1665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:LG110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="KI1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="LG49" sqref="LG49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2928,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -7723,7 +7726,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -9624,7 +9627,7 @@
         <v>0</v>
       </c>
       <c r="LG8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:319">
@@ -10553,10 +10556,10 @@
         <v>0</v>
       </c>
       <c r="KW9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY9" s="2">
         <v>0</v>
@@ -11542,7 +11545,7 @@
         <v>0</v>
       </c>
       <c r="LG10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:319">
@@ -17266,10 +17269,10 @@
         <v>0</v>
       </c>
       <c r="KW16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY16" s="2">
         <v>0</v>
@@ -18225,10 +18228,10 @@
         <v>0</v>
       </c>
       <c r="KW17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY17" s="2">
         <v>0</v>
@@ -23020,10 +23023,10 @@
         <v>0</v>
       </c>
       <c r="KW22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY22" s="2">
         <v>0</v>
@@ -24026,7 +24029,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
@@ -24968,7 +24971,7 @@
         <v>0</v>
       </c>
       <c r="LG24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:319">
@@ -32610,10 +32613,10 @@
         <v>0</v>
       </c>
       <c r="KW32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY32" s="2">
         <v>0</v>
@@ -34528,10 +34531,10 @@
         <v>0</v>
       </c>
       <c r="KW34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY34" s="2">
         <v>0</v>
@@ -35487,10 +35490,10 @@
         <v>0</v>
       </c>
       <c r="KW35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY35" s="2">
         <v>0</v>
@@ -35517,7 +35520,7 @@
         <v>0</v>
       </c>
       <c r="LG35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:319">
@@ -37405,10 +37408,10 @@
         <v>0</v>
       </c>
       <c r="KW37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY37" s="2">
         <v>0</v>
@@ -39323,10 +39326,10 @@
         <v>0</v>
       </c>
       <c r="KW39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY39" s="2">
         <v>0</v>
@@ -40282,10 +40285,10 @@
         <v>0</v>
       </c>
       <c r="KW40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY40" s="2">
         <v>0</v>
@@ -43189,7 +43192,7 @@
         <v>0</v>
       </c>
       <c r="LG43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:319">
@@ -47954,10 +47957,10 @@
         <v>0</v>
       </c>
       <c r="KW48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY48" s="2">
         <v>0</v>
@@ -58503,10 +58506,10 @@
         <v>0</v>
       </c>
       <c r="KW59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY59" s="2">
         <v>0</v>
@@ -60468,7 +60471,7 @@
         <v>0</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
@@ -61380,10 +61383,10 @@
         <v>0</v>
       </c>
       <c r="KW62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY62" s="2">
         <v>0</v>
@@ -64257,10 +64260,10 @@
         <v>0</v>
       </c>
       <c r="KW65" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KX65" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KY65" s="2">
         <v>0</v>
@@ -66175,10 +66178,10 @@
         <v>0</v>
       </c>
       <c r="KW67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY67" s="2">
         <v>0</v>
@@ -70011,10 +70014,10 @@
         <v>0</v>
       </c>
       <c r="KW71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY71" s="2">
         <v>0</v>
@@ -76724,10 +76727,10 @@
         <v>0</v>
       </c>
       <c r="KW78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX78" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY78" s="2">
         <v>0</v>
@@ -80560,10 +80563,10 @@
         <v>0</v>
       </c>
       <c r="KW82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX82" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY82" s="2">
         <v>0</v>
@@ -80607,7 +80610,7 @@
         <v>0</v>
       </c>
       <c r="E83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="2">
         <v>1</v>
@@ -81519,10 +81522,10 @@
         <v>0</v>
       </c>
       <c r="KW83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX83" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY83" s="2">
         <v>0</v>
@@ -86314,10 +86317,10 @@
         <v>0</v>
       </c>
       <c r="KW88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX88" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY88" s="2">
         <v>0</v>
@@ -86361,7 +86364,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" s="2">
         <v>0</v>
@@ -87273,10 +87276,10 @@
         <v>0</v>
       </c>
       <c r="KW89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY89" s="2">
         <v>0</v>
@@ -91156,7 +91159,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="2">
         <v>0</v>
@@ -102617,10 +102620,10 @@
         <v>0</v>
       </c>
       <c r="KW105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX105" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KY105" s="2">
         <v>0</v>
@@ -107446,6 +107449,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:LG110"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>